<commit_message>
Add SRS review sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/SRS_Review.xlsx
+++ b/Software Specifications/SRS/SRS_Review.xlsx
@@ -159,7 +159,7 @@
   </si>
   <si>
     <t xml:space="preserve">Instead of saying this function shall xxxxx , you could say the SW shall do xxxxxxx as all of those requirements in SRS 
-describe how the sw shall handle the system functionalities. </t>
+describe how the sw shall handle the system functionalities.</t>
   </si>
   <si>
     <t xml:space="preserve">You need to change the requirement ID numbers as it should use only integer numbers for each separate requirement.</t>
@@ -209,7 +209,7 @@
     <numFmt numFmtId="168" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -254,12 +254,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -444,7 +438,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -545,18 +539,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,7 +567,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,7 +575,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,7 +680,7 @@
       <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.27"/>
   </cols>
@@ -935,10 +921,10 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.72"/>
@@ -1046,7 +1032,7 @@
       <c r="E4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="24"/>
@@ -1071,7 +1057,7 @@
       <c r="E5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="23" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="24"/>
@@ -1096,7 +1082,7 @@
       <c r="E6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="23" t="s">
         <v>35</v>
       </c>
       <c r="G6" s="24"/>
@@ -1121,7 +1107,7 @@
       <c r="E7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="23" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="24"/>
@@ -1146,7 +1132,7 @@
       <c r="E8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>39</v>
       </c>
       <c r="G8" s="24"/>
@@ -1171,7 +1157,7 @@
       <c r="E9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="24"/>
@@ -1187,7 +1173,7 @@
       <c r="B10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -1196,7 +1182,7 @@
       <c r="E10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="24"/>
@@ -1215,7 +1201,7 @@
       <c r="B11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -1239,10 +1225,10 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
-      <c r="C12" s="27"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="20"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="28"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24" t="s">
         <v>28</v>
@@ -1255,7 +1241,7 @@
       <c r="C13" s="21"/>
       <c r="D13" s="20"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="26"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
@@ -1269,7 +1255,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="20"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="22"/>
@@ -1283,7 +1269,7 @@
       <c r="C15" s="21"/>
       <c r="D15" s="20"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="22"/>
@@ -1294,7 +1280,7 @@
       <c r="C16" s="21"/>
       <c r="D16" s="20"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="26"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="22"/>
@@ -1305,7 +1291,7 @@
       <c r="C17" s="21"/>
       <c r="D17" s="20"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="26"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="22"/>
@@ -1322,7 +1308,7 @@
       <c r="C18" s="21"/>
       <c r="D18" s="20"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="22"/>
@@ -1339,7 +1325,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="20"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="22"/>
@@ -1350,7 +1336,7 @@
       <c r="C20" s="21"/>
       <c r="D20" s="20"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="22"/>
@@ -1361,362 +1347,362 @@
       <c r="C21" s="21"/>
       <c r="D21" s="20"/>
       <c r="E21" s="22"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="20"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="34"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="34"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="20"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
-      <c r="I28" s="34"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
-      <c r="I29" s="34"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="I30" s="34"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="20"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
-      <c r="I31" s="34"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="20"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="34"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="20"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
-      <c r="I33" s="34"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="36"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="34"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="36"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
-      <c r="I35" s="34"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
-      <c r="I36" s="34"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="37"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
-      <c r="I37" s="34"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="36"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
-      <c r="I38" s="34"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="36"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="34"/>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>
-      <c r="I39" s="34"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="34"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="36"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="34"/>
       <c r="G41" s="24"/>
       <c r="H41" s="24"/>
-      <c r="I41" s="34"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="36"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="34"/>
       <c r="G42" s="24"/>
       <c r="H42" s="24"/>
-      <c r="I42" s="34"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="36"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="34"/>
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
-      <c r="I43" s="34"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="36"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
-      <c r="I44" s="34"/>
+      <c r="I44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="36"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="34"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
-      <c r="I45" s="34"/>
+      <c r="I45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="36"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="34"/>
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
-      <c r="I46" s="34"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="36"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="34"/>
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
-      <c r="I47" s="34"/>
+      <c r="I47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="36"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="34"/>
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
-      <c r="I48" s="34"/>
+      <c r="I48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="36"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="34"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
-      <c r="I49" s="34"/>
+      <c r="I49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="36"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="34"/>
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
-      <c r="I50" s="34"/>
+      <c r="I50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="36"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="34"/>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
-      <c r="I51" s="34"/>
+      <c r="I51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="36"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="34"/>
       <c r="G52" s="24"/>
       <c r="H52" s="24"/>
-      <c r="I52" s="34"/>
+      <c r="I52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="31"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="36"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="34"/>
       <c r="G53" s="24"/>
       <c r="H53" s="24"/>
-      <c r="I53" s="34"/>
+      <c r="I53" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">

</xml_diff>